<commit_message>
[weekly] Upgrade purchase analyze
</commit_message>
<xml_diff>
--- a/support_data/purchase_analysis/summary_row.xlsx
+++ b/support_data/purchase_analysis/summary_row.xlsx
@@ -439,31 +439,31 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>43950</v>
+        <v>43963</v>
       </c>
       <c r="B2" s="2">
-        <v>43963</v>
+        <v>43971</v>
       </c>
       <c r="C2">
-        <v>309130.009</v>
+        <v>1401065.028</v>
       </c>
       <c r="D2">
-        <v>119071.213</v>
+        <v>119239.422</v>
       </c>
       <c r="E2">
-        <v>229007.88</v>
+        <v>600189.9199999999</v>
       </c>
       <c r="F2">
-        <v>113207.88</v>
+        <v>89747.91</v>
       </c>
       <c r="G2">
-        <v>110968.3719999999</v>
+        <v>830812.4570000001</v>
       </c>
       <c r="H2">
-        <v>132647.813</v>
+        <v>244402.9349999999</v>
       </c>
       <c r="I2">
-        <v>0.6410300884117661</v>
+        <v>0.4070136357725145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[master] Current status 29/01/2021
</commit_message>
<xml_diff>
--- a/support_data/purchase_analysis/summary_row.xlsx
+++ b/support_data/purchase_analysis/summary_row.xlsx
@@ -439,31 +439,31 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>43963</v>
+        <v>44207</v>
       </c>
       <c r="B2" s="2">
-        <v>43971</v>
+        <v>44216</v>
       </c>
       <c r="C2">
-        <v>1401065.028</v>
+        <v>727695.1500000001</v>
       </c>
       <c r="D2">
-        <v>119239.422</v>
+        <v>88097.13499999998</v>
       </c>
       <c r="E2">
-        <v>600189.9199999999</v>
+        <v>496711.2499999999</v>
       </c>
       <c r="F2">
-        <v>89747.91</v>
+        <v>403027.01</v>
       </c>
       <c r="G2">
-        <v>830812.4570000001</v>
+        <v>675741.05</v>
       </c>
       <c r="H2">
-        <v>244402.9349999999</v>
+        <v>131857.4809999999</v>
       </c>
       <c r="I2">
-        <v>0.4070136357725145</v>
+        <v>0.07139541880964863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>